<commit_message>
few modifications for no data screen
</commit_message>
<xml_diff>
--- a/backend/income_details.xlsx
+++ b/backend/income_details.xlsx
@@ -397,124 +397,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>Source</v>
-      </c>
-      <c r="B1" t="str">
-        <v>Amount</v>
-      </c>
-      <c r="C1" t="str">
-        <v>Date</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>property profit</v>
-      </c>
-      <c r="B2">
-        <v>3</v>
-      </c>
-      <c r="C2" t="str">
-        <v>2026-01-21</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>chill</v>
-      </c>
-      <c r="B3">
-        <v>1000</v>
-      </c>
-      <c r="C3" t="str">
-        <v>2025-07-27</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>d</v>
-      </c>
-      <c r="B4">
-        <v>10</v>
-      </c>
-      <c r="C4" t="str">
-        <v>2025-07-24</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>stocks</v>
-      </c>
-      <c r="B5">
-        <v>88998</v>
-      </c>
-      <c r="C5" t="str">
-        <v>2025-07-24</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>intrest</v>
-      </c>
-      <c r="B6">
-        <v>300000</v>
-      </c>
-      <c r="C6" t="str">
-        <v>2025-06-27</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>sotcks</v>
-      </c>
-      <c r="B7">
-        <v>8000</v>
-      </c>
-      <c r="C7" t="str">
-        <v>2025-06-15</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="str">
-        <v>intern</v>
-      </c>
-      <c r="B8">
-        <v>60000</v>
-      </c>
-      <c r="C8" t="str">
-        <v>2025-06-15</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="str">
-        <v>farm income</v>
-      </c>
-      <c r="B9">
-        <v>100000</v>
-      </c>
-      <c r="C9" t="str">
-        <v>2025-05-24</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="str">
-        <v>rental income</v>
-      </c>
-      <c r="B10">
-        <v>100000</v>
-      </c>
-      <c r="C10" t="str">
-        <v>2025-02-24</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C10"/>
+    <ignoredError numberStoredAsText="1" sqref="A1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>